<commit_message>
Polish Category Bulk Import
</commit_message>
<xml_diff>
--- a/public/download/category_bulk_demo.xlsx
+++ b/public/download/category_bulk_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laravel\e-commerce\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B7B22D-A355-44B4-9459-06E1DA978E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A115EBCC-E8A3-46F7-BBDB-61DE0D019AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>https://adyanmart.s3.ap-southeast-1.amazonaws.com/uploads/products/thumbnail/ZJqm0yHhBrLD7Zn2Wbtw6nkKxKtB9xntMh8ON8D1.jpeg</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Buy monitor in Bangladesh with the best price</t>
   </si>
   <si>
-    <t>Buy Monitor at best price</t>
-  </si>
-  <si>
     <t>site_title</t>
   </si>
   <si>
@@ -90,18 +84,9 @@
     <t>Buy monitor in bangldesh</t>
   </si>
   <si>
-    <t>meta_article_tag</t>
-  </si>
-  <si>
-    <t>meta_script_tag</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>featured</t>
   </si>
   <si>
@@ -118,9 +103,6 @@
   </si>
   <si>
     <t>Buy Dell monitor in Bangladesh</t>
-  </si>
-  <si>
-    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -457,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,20 +451,18 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="12" width="23.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="126.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="126.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -491,127 +471,111 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>